<commit_message>
incorporated edits from 2nd round of peer review, finalized data files for upload to SeaBASS (NASA repository)
</commit_message>
<xml_diff>
--- a/data/MOCNESS_data/MOCNESS 1 Cook/Ecotaxa_small_Cook_fish/Ecotaxa_small_fish_Cook_red_delete_green_add_yellow_edit.xlsx
+++ b/data/MOCNESS_data/MOCNESS 1 Cook/Ecotaxa_small_Cook_fish/Ecotaxa_small_fish_Cook_red_delete_green_add_yellow_edit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hmcmonag/Desktop/Chapter-2/Chapter-2-Fish-carbon-flux-N-Atlantic/data/MOCNESS_data/MOCNESS 1 Cook/Ecotaxa_small_Cook_fish/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hmcmonag/Desktop/Chapter-2-public-repo/Fish-carbon-N-Atlantic/data/MOCNESS_data/MOCNESS 1 Cook/Ecotaxa_small_Cook_fish/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A551AA-125A-8B49-B337-5F3A2CA30607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C0EAAD-3CFC-894C-A28E-6C3AC232968B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31360" yWindow="500" windowWidth="37160" windowHeight="17280" xr2:uid="{90454835-96B0-7D49-8D3C-5234412AA662}"/>
+    <workbookView xWindow="1560" yWindow="1600" windowWidth="28560" windowHeight="16700" xr2:uid="{90454835-96B0-7D49-8D3C-5234412AA662}"/>
   </bookViews>
   <sheets>
     <sheet name="Ecotaxa_small_fish_Cook" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="102">
   <si>
     <t>Tow_number</t>
   </si>
@@ -293,13 +293,46 @@
   </si>
   <si>
     <t>209010_2000_1_8_1_tot_1_170</t>
+  </si>
+  <si>
+    <t>deleted</t>
+  </si>
+  <si>
+    <t>added</t>
+  </si>
+  <si>
+    <t>Added to SeaBASS and final Ecotaxa_small_fish_Cook file?</t>
+  </si>
+  <si>
+    <t>was already in these files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edited from Paralepididae to Teleostei in Ecotaxa_small_fish_Cook. left out of SeaBASS because unidentified to family and not used in final analysis. </t>
+  </si>
+  <si>
+    <t>added (and calculated estimated weight to add to SeaBASS)</t>
+  </si>
+  <si>
+    <t>was highlighted because splits should be 1. Hadn't been added to Ecotaxa_small_fish_Cook. Added now. Deleted extra rows in SeaBASS because (see highlighted yellow) this was not from a split.</t>
+  </si>
+  <si>
+    <t>was already in Ecotaxa_small_fish_Cook. not adding to seabass because paralepididae aren't included in final analysis</t>
+  </si>
+  <si>
+    <t>highlighted because splits should be 1. Hadn't been added to Ecotaxa_small_fish_Cook. Added now. Fixed replicate rows in SeaBASS to include just 1 row because this did not come from a split sample.</t>
+  </si>
+  <si>
+    <t>added to Ecotaxa_small_fish_Cook.</t>
+  </si>
+  <si>
+    <t>was already in Ecotaxa_small_fish_Cook. added to SeaBASS (4 columns, because fish was from a quarter split)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -447,8 +480,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Aptos Narrow (Body)"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -646,6 +683,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -807,13 +850,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1195,10 +1240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C853EDD9-9C07-1D48-B481-09635CABF96C}">
-  <dimension ref="A1:Z54"/>
+  <dimension ref="A1:AA54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="Q39" sqref="Q39"/>
+    <sheetView tabSelected="1" topLeftCell="T31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Z42" sqref="Z42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1206,7 +1251,7 @@
     <col min="26" max="26" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1285,8 +1330,11 @@
       <c r="Z1" t="s">
         <v>25</v>
       </c>
+      <c r="AA1" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10</v>
       </c>
@@ -1365,8 +1413,11 @@
       <c r="Z2" t="s">
         <v>31</v>
       </c>
+      <c r="AA2" t="s">
+        <v>94</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>10</v>
       </c>
@@ -1445,8 +1496,11 @@
       <c r="Z3" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="AA3" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>11</v>
       </c>
@@ -1525,8 +1579,11 @@
       <c r="Z4" t="s">
         <v>35</v>
       </c>
+      <c r="AA4" t="s">
+        <v>95</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>11</v>
       </c>
@@ -1605,8 +1662,11 @@
       <c r="Z5" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="AA5" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="6" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>11</v>
       </c>
@@ -1685,8 +1745,11 @@
       <c r="Z6" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="AA6" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="7" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>11</v>
       </c>
@@ -1765,8 +1828,11 @@
       <c r="Z7" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="AA7" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="8" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>11</v>
       </c>
@@ -1845,8 +1911,11 @@
       <c r="Z8" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="AA8" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="9" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>11</v>
       </c>
@@ -1925,8 +1994,11 @@
       <c r="Z9" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="AA9" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="10" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>11</v>
       </c>
@@ -2005,8 +2077,11 @@
       <c r="Z10" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="AA10" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="11" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>11</v>
       </c>
@@ -2085,8 +2160,11 @@
       <c r="Z11" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="AA11" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="12" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2165,8 +2243,11 @@
       <c r="Z12" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="AA12" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="13" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -2245,8 +2326,11 @@
       <c r="Z13" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="AA13" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="14" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -2325,8 +2409,11 @@
       <c r="Z14" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="AA14" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="15" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>11</v>
       </c>
@@ -2405,8 +2492,11 @@
       <c r="Z15" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="AA15" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="16" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>11</v>
       </c>
@@ -2485,8 +2575,11 @@
       <c r="Z16" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="AA16" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="17" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>11</v>
       </c>
@@ -2565,8 +2658,11 @@
       <c r="Z17" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="AA17" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="18" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>11</v>
       </c>
@@ -2645,8 +2741,11 @@
       <c r="Z18" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="AA18" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="19" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>11</v>
       </c>
@@ -2725,8 +2824,11 @@
       <c r="Z19" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="AA19" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="20" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>11</v>
       </c>
@@ -2805,8 +2907,11 @@
       <c r="Z20" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="AA20" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="21" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>11</v>
       </c>
@@ -2885,8 +2990,11 @@
       <c r="Z21" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="AA21" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="22" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>11</v>
       </c>
@@ -2965,8 +3073,11 @@
       <c r="Z22" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="AA22" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="23" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>11</v>
       </c>
@@ -3045,8 +3156,11 @@
       <c r="Z23" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="AA23" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="24" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>11</v>
       </c>
@@ -3125,8 +3239,11 @@
       <c r="Z24" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="AA24" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="25" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>11</v>
       </c>
@@ -3205,8 +3322,11 @@
       <c r="Z25" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="AA25" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="26" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>11</v>
       </c>
@@ -3285,8 +3405,11 @@
       <c r="Z26" s="2" t="s">
         <v>58</v>
       </c>
+      <c r="AA26" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="27" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>11</v>
       </c>
@@ -3365,8 +3488,11 @@
       <c r="Z27" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="AA27" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="28" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>11</v>
       </c>
@@ -3445,8 +3571,11 @@
       <c r="Z28" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="AA28" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="29" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>11</v>
       </c>
@@ -3525,8 +3654,11 @@
       <c r="Z29" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="AA29" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="30" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>11</v>
       </c>
@@ -3605,8 +3737,11 @@
       <c r="Z30" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="AA30" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="31" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>11</v>
       </c>
@@ -3685,8 +3820,11 @@
       <c r="Z31" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AA31" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="32" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>11</v>
       </c>
@@ -3765,8 +3903,11 @@
       <c r="Z32" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="AA32" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="33" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>11</v>
       </c>
@@ -3845,8 +3986,11 @@
       <c r="Z33" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="AA33" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="34" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>11</v>
       </c>
@@ -3925,8 +4069,11 @@
       <c r="Z34" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="AA34" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="35" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>11</v>
       </c>
@@ -4005,8 +4152,11 @@
       <c r="Z35" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="AA35" s="1" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="36" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>11</v>
       </c>
@@ -4085,8 +4235,11 @@
       <c r="Z36" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="AA36" s="1" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>48</v>
       </c>
@@ -4165,8 +4318,11 @@
       <c r="Z37" t="s">
         <v>67</v>
       </c>
+      <c r="AA37" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>48</v>
       </c>
@@ -4245,8 +4401,11 @@
       <c r="Z38" t="s">
         <v>68</v>
       </c>
+      <c r="AA38" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>48</v>
       </c>
@@ -4325,8 +4484,11 @@
       <c r="Z39" t="s">
         <v>69</v>
       </c>
+      <c r="AA39" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="40" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>89</v>
       </c>
@@ -4405,8 +4567,11 @@
       <c r="Z40" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="AA40" s="7" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="41" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>89</v>
       </c>
@@ -4485,8 +4650,11 @@
       <c r="Z41" s="1" t="s">
         <v>86</v>
       </c>
+      <c r="AA41" s="6" t="s">
+        <v>92</v>
+      </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>90</v>
       </c>
@@ -4565,8 +4733,11 @@
       <c r="Z42" t="s">
         <v>70</v>
       </c>
+      <c r="AA42" t="s">
+        <v>99</v>
+      </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>90</v>
       </c>
@@ -4645,8 +4816,11 @@
       <c r="Z43" t="s">
         <v>71</v>
       </c>
+      <c r="AA43" t="s">
+        <v>99</v>
+      </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>90</v>
       </c>
@@ -4725,8 +4899,11 @@
       <c r="Z44" t="s">
         <v>72</v>
       </c>
+      <c r="AA44" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>90</v>
       </c>
@@ -4805,8 +4982,11 @@
       <c r="Z45" t="s">
         <v>73</v>
       </c>
+      <c r="AA45" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>90</v>
       </c>
@@ -4885,8 +5065,11 @@
       <c r="Z46" t="s">
         <v>74</v>
       </c>
+      <c r="AA46" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>90</v>
       </c>
@@ -4965,8 +5148,11 @@
       <c r="Z47" t="s">
         <v>75</v>
       </c>
+      <c r="AA47" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>90</v>
       </c>
@@ -5045,8 +5231,11 @@
       <c r="Z48" t="s">
         <v>76</v>
       </c>
+      <c r="AA48" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="49" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>90</v>
       </c>
@@ -5125,8 +5314,11 @@
       <c r="Z49" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="AA49" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="50" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>90</v>
       </c>
@@ -5205,8 +5397,11 @@
       <c r="Z50" s="3" t="s">
         <v>87</v>
       </c>
+      <c r="AA50" s="1" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="51" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>90</v>
       </c>
@@ -5285,8 +5480,11 @@
       <c r="Z51" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="AA51" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="52" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>90</v>
       </c>
@@ -5365,8 +5563,11 @@
       <c r="Z52" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="AA52" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>48</v>
       </c>
@@ -5445,8 +5646,11 @@
       <c r="Z53" t="s">
         <v>77</v>
       </c>
+      <c r="AA53" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>48</v>
       </c>
@@ -5524,6 +5728,9 @@
       </c>
       <c r="Z54" t="s">
         <v>78</v>
+      </c>
+      <c r="AA54" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>